<commit_message>
fix typo + add option to skip prt linking
</commit_message>
<xml_diff>
--- a/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_TEMPLATE.xlsx
+++ b/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_TEMPLATE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
   <si>
     <t>Value</t>
   </si>
@@ -389,6 +389,15 @@
   </si>
   <si>
     <t>Use absolute paths in multi-participant MDMs</t>
+  </si>
+  <si>
+    <t>VTC.LINK_PRT</t>
+  </si>
+  <si>
+    <t>This step is recommended, but you could disable it to save time if the linking has already been performed.</t>
+  </si>
+  <si>
+    <t>Link PRT to VTCs</t>
   </si>
 </sst>
 </file>
@@ -432,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -452,6 +461,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -510,8 +522,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E29" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E30" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E30"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Category" dataDxfId="4"/>
     <tableColumn id="5" name="Description" dataDxfId="3"/>
@@ -812,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,12 +1208,20 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
+      <c r="B30" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>

</xml_diff>

<commit_message>
added option to skip vtc checks
</commit_message>
<xml_diff>
--- a/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_TEMPLATE.xlsx
+++ b/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_TEMPLATE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
   <si>
     <t>Value</t>
   </si>
@@ -398,6 +398,15 @@
   </si>
   <si>
     <t>Link PRT to VTCs</t>
+  </si>
+  <si>
+    <t>Check VTC TR and Volumes</t>
+  </si>
+  <si>
+    <t>This step is recommended, but you could disable it to save time it has already been performed.</t>
+  </si>
+  <si>
+    <t>VTC.CHECK</t>
   </si>
 </sst>
 </file>
@@ -522,8 +531,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E30" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E31" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E31"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Category" dataDxfId="4"/>
     <tableColumn id="5" name="Description" dataDxfId="3"/>
@@ -825,7 +834,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,12 +1232,20 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
+      <c r="B31" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>

</xml_diff>

<commit_message>
add option to overwrite prt
</commit_message>
<xml_diff>
--- a/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_TEMPLATE.xlsx
+++ b/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_TEMPLATE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
   <si>
     <t>Value</t>
   </si>
@@ -407,6 +407,15 @@
   </si>
   <si>
     <t>VTC.CHECK</t>
+  </si>
+  <si>
+    <t>PRT Overwrite</t>
+  </si>
+  <si>
+    <t>PRT.OVERWRITE</t>
+  </si>
+  <si>
+    <t>When copying PRT, overwrite existing files.</t>
   </si>
 </sst>
 </file>
@@ -833,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,10 +1265,18 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
+      <c r="B33" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>

</xml_diff>

<commit_message>
support wildcard * in VTC.NAME
</commit_message>
<xml_diff>
--- a/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_TEMPLATE.xlsx
+++ b/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_TEMPLATE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>Value</t>
   </si>
@@ -416,6 +416,9 @@
   </si>
   <si>
     <t>When copying PRT, overwrite existing files.</t>
+  </si>
+  <si>
+    <t>Name entered in the Create Document Workflow. May include wildcard (*).</t>
   </si>
 </sst>
 </file>
@@ -842,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,7 +1012,7 @@
         <v>37</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
post-preprocessing - added func res check
</commit_message>
<xml_diff>
--- a/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_TEMPLATE.xlsx
+++ b/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_TEMPLATE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
   <si>
     <t>Value</t>
   </si>
@@ -419,6 +419,12 @@
   </si>
   <si>
     <t>This step is recommended, but you could disable it to save time if it has already been performed.</t>
+  </si>
+  <si>
+    <t>EXP.RES</t>
+  </si>
+  <si>
+    <t>Functional resolution in mm.</t>
   </si>
 </sst>
 </file>
@@ -543,8 +549,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E31" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E32" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E32"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Category" dataDxfId="4"/>
     <tableColumn id="5" name="Description" dataDxfId="3"/>
@@ -843,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,210 +1089,216 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
+      <c r="B18" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="C18" s="6"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="D18" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C20" s="6">
         <v>2</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C22" s="6">
         <v>6</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D22" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="5" t="s">
+      <c r="C26" s="7"/>
+      <c r="D26" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-    </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B28" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="6" t="b">
+      <c r="C28" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="6" t="b">
+      <c r="C30" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D30" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C31" s="6" t="b">
         <v>1</v>
       </c>
       <c r="D31" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E32" s="5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
-      <c r="B33" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C33" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>84</v>
-      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
+      <c r="B34" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
@@ -1308,6 +1320,13 @@
       <c r="C37" s="6"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added new field to skip BBR checks
</commit_message>
<xml_diff>
--- a/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_TEMPLATE.xlsx
+++ b/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_TEMPLATE.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="93">
   <si>
     <t>Value</t>
   </si>
@@ -425,6 +425,28 @@
   </si>
   <si>
     <t>Functional resolution in mm.</t>
+  </si>
+  <si>
+    <t>FMR.BBR</t>
+  </si>
+  <si>
+    <t>Check BBR Values</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Read text files in "_WorkflowReports_\texts" to evaluate the success of Boundary-Based Registration (FMR-VMR Coregistration) for each run. The results are displayed in the Command Window as well as written to the log file. BBR was the default option in BV20, but BV21 now defaults to use the NGF method instead so the new default is FALSE. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Set TRUE if you used BBR for FMR-VMR Coregistration.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -605,7 +627,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -640,7 +662,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -851,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,12 +1329,20 @@
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
+      <c r="B36" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>

</xml_diff>

<commit_message>
add support for custom run names
</commit_message>
<xml_diff>
--- a/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_TEMPLATE.xlsx
+++ b/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_TEMPLATE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="97">
   <si>
     <t>Value</t>
   </si>
@@ -447,6 +447,31 @@
       </rPr>
       <t>Set TRUE if you used BBR for FMR-VMR Coregistration.</t>
     </r>
+  </si>
+  <si>
+    <t>Run Names</t>
+  </si>
+  <si>
+    <t>[FuncName]-S1R[R#1]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When entered correctly, BV should name runs in the format of "[FuncName]-S1R[R#1]". </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>This field accomodates other run naming schemes, but can typically be left as the default.</t>
+    </r>
+  </si>
+  <si>
+    <t>RUN.NAME_FORMAT</t>
   </si>
 </sst>
 </file>
@@ -571,8 +596,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E32" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E33" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E33"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Category" dataDxfId="4"/>
     <tableColumn id="5" name="Description" dataDxfId="3"/>
@@ -871,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,7 +908,7 @@
     <col min="2" max="2" width="73.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="50.5703125" customWidth="1"/>
     <col min="4" max="4" width="74.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1046,310 +1071,318 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="B13" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="5" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="6" t="b">
-        <v>0</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C17" s="6"/>
       <c r="D17" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" s="6"/>
+        <v>55</v>
+      </c>
+      <c r="C18" s="6" t="b">
+        <v>0</v>
+      </c>
       <c r="D18" s="5" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
+      <c r="B19" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="C19" s="6"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="D19" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C21" s="6">
         <v>2</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E21" s="5" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C23" s="6">
         <v>6</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="5" t="s">
+      <c r="C27" s="7"/>
+      <c r="D27" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-    </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B29" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="6" t="b">
+      <c r="C29" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D29" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B31" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C30" s="6" t="b">
+      <c r="C31" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D31" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E31" s="5" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C32" s="6" t="b">
         <v>1</v>
       </c>
       <c r="D32" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E33" s="5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
-      <c r="B34" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C34" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>84</v>
-      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="5"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C36" s="6" t="b">
+      <c r="C37" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D37" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E37" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
@@ -1357,6 +1390,13 @@
       <c r="C38" s="6"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>